<commit_message>
Add support for XRechnung 3.0; TICC-290; TICC-291
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Document types v8.7.xlsx
+++ b/work-in-progress/Peppol Code Lists - Document types v8.7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31243315-2F80-4B53-B281-41CF9E663B16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB89C29-9761-43C3-96BF-F1722A545D5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1818" uniqueCount="641">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1866" uniqueCount="655">
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ApplicationResponse-2::ApplicationResponse##urn:www.cenbii.eu:transaction:biicoretrdm057:ver1.0:#urn:www.peppol.eu:bis:peppol1a:ver1.0::2.0</t>
   </si>
@@ -2010,6 +2010,48 @@
   <si>
     <t>TICC-107
 TICC-287</t>
+  </si>
+  <si>
+    <t>XRechnung UBL Invoice V3.0</t>
+  </si>
+  <si>
+    <t>XRechnung UBL CreditNote V3.0</t>
+  </si>
+  <si>
+    <t>XRechnung CII Invoice V3.0</t>
+  </si>
+  <si>
+    <t>XRechnung UBL Invoice V3.0 Extension</t>
+  </si>
+  <si>
+    <t>XRechnung UBL CreditNote V3.0 Extension</t>
+  </si>
+  <si>
+    <t>XRechnung CII Invoice V3.0 Extension</t>
+  </si>
+  <si>
+    <t>TICC-291</t>
+  </si>
+  <si>
+    <t>TICC-290</t>
+  </si>
+  <si>
+    <t>urn:un:unece:uncefact:data:standard:CrossIndustryInvoice:100::CrossIndustryInvoice##urn:cen.eu:en16931:2017#compliant#urn:xeinkauf.de:kosit:xrechnung_3.0#conformant#urn:xeinkauf.de:kosit:extension:xrechnung_3.0::D16B</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:CreditNote-2::CreditNote##urn:cen.eu:en16931:2017#compliant#urn:xeinkauf.de:kosit:xrechnung_3.0#conformant#urn:xeinkauf. de:kosit:extension:xrechnung_3.0::2.1</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:Invoice-2::Invoice##urn:cen.eu:en16931:2017#compliant#urn:xeinkauf.de:kosit:xrechnung_3.0#conformant#urn:xeinkauf. de:kosit:extension:xrechnung_3.0::2.1</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:Invoice-2::Invoice##urn:cen.eu:en16931:2017#compliant#urn:xeinkauf.de:kosit:xrechnung_3.0::2.1</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:CreditNote-2::CreditNote##urn:cen.eu:en16931:2017#compliant#urn:xeinkauf.de:kosit:xrechnung_3.0::2.1</t>
+  </si>
+  <si>
+    <t>urn:un:unece:uncefact:data:standard:CrossIndustryInvoice:100::CrossIndustryInvoice##urn:cen.eu:en16931:2017#compliant#urn:xeinkauf.de:kosit:xrechnung_3.0::D16B</t>
   </si>
 </sst>
 </file>
@@ -2669,11 +2711,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F45987FB-91F4-488D-A9D3-2F3FAED3E07C}">
-  <dimension ref="A1:L237"/>
+  <dimension ref="A1:L243"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C76" sqref="C76"/>
+      <pane ySplit="1" topLeftCell="A230" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C241" sqref="C241"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10228,6 +10270,180 @@
         <v>538</v>
       </c>
     </row>
+    <row r="238" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A238" s="5" t="s">
+        <v>641</v>
+      </c>
+      <c r="B238" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C238" s="5" t="s">
+        <v>652</v>
+      </c>
+      <c r="D238" s="29" t="s">
+        <v>639</v>
+      </c>
+      <c r="E238" s="24" t="s">
+        <v>368</v>
+      </c>
+      <c r="H238" s="5" t="s">
+        <v>647</v>
+      </c>
+      <c r="I238" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K238" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="L238" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="239" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A239" s="5" t="s">
+        <v>642</v>
+      </c>
+      <c r="B239" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C239" s="5" t="s">
+        <v>653</v>
+      </c>
+      <c r="D239" s="29" t="s">
+        <v>639</v>
+      </c>
+      <c r="E239" s="24" t="s">
+        <v>368</v>
+      </c>
+      <c r="H239" s="5" t="s">
+        <v>647</v>
+      </c>
+      <c r="I239" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K239" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="L239" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="240" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A240" s="5" t="s">
+        <v>643</v>
+      </c>
+      <c r="B240" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C240" s="5" t="s">
+        <v>654</v>
+      </c>
+      <c r="D240" s="29" t="s">
+        <v>639</v>
+      </c>
+      <c r="E240" s="24" t="s">
+        <v>368</v>
+      </c>
+      <c r="H240" s="5" t="s">
+        <v>647</v>
+      </c>
+      <c r="I240" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K240" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="L240" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="241" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A241" s="5" t="s">
+        <v>644</v>
+      </c>
+      <c r="B241" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C241" s="5" t="s">
+        <v>651</v>
+      </c>
+      <c r="D241" s="29" t="s">
+        <v>639</v>
+      </c>
+      <c r="E241" s="24" t="s">
+        <v>368</v>
+      </c>
+      <c r="H241" s="5" t="s">
+        <v>648</v>
+      </c>
+      <c r="I241" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K241" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="L241" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="242" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A242" s="5" t="s">
+        <v>645</v>
+      </c>
+      <c r="B242" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C242" s="5" t="s">
+        <v>650</v>
+      </c>
+      <c r="D242" s="29" t="s">
+        <v>639</v>
+      </c>
+      <c r="E242" s="24" t="s">
+        <v>368</v>
+      </c>
+      <c r="H242" s="5" t="s">
+        <v>648</v>
+      </c>
+      <c r="I242" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K242" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="L242" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="243" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A243" s="5" t="s">
+        <v>646</v>
+      </c>
+      <c r="B243" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C243" s="5" t="s">
+        <v>649</v>
+      </c>
+      <c r="D243" s="29" t="s">
+        <v>639</v>
+      </c>
+      <c r="E243" s="24" t="s">
+        <v>368</v>
+      </c>
+      <c r="H243" s="5" t="s">
+        <v>648</v>
+      </c>
+      <c r="I243" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K243" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="L243" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:L237" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added SG PINT Invoice and CreditNote; TICC-297
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Document types v8.7.xlsx
+++ b/work-in-progress/Peppol Code Lists - Document types v8.7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB89C29-9761-43C3-96BF-F1722A545D5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56ADEEA8-57DA-47CF-AFF4-B9CDDD742FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Document Type" sheetId="5" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Document Type'!$A$1:$L$237</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Document Type'!$A$1:$L$245</definedName>
     <definedName name="_ftn1" localSheetId="0">'Document Type'!#REF!</definedName>
     <definedName name="_ftn2" localSheetId="0">'Document Type'!#REF!</definedName>
     <definedName name="_ftn3" localSheetId="0">'Document Type'!#REF!</definedName>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1866" uniqueCount="655">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1882" uniqueCount="660">
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ApplicationResponse-2::ApplicationResponse##urn:www.cenbii.eu:transaction:biicoretrdm057:ver1.0:#urn:www.peppol.eu:bis:peppol1a:ver1.0::2.0</t>
   </si>
@@ -2052,6 +2052,21 @@
   </si>
   <si>
     <t>urn:un:unece:uncefact:data:standard:CrossIndustryInvoice:100::CrossIndustryInvoice##urn:cen.eu:en16931:2017#compliant#urn:xeinkauf.de:kosit:xrechnung_3.0::D16B</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:Invoice-2::Invoice##urn:peppol:pint:billing-1@sg-1::2.1</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:CreditNote-2::CreditNote##urn:peppol:pint:billing-1@sg-1::2.1</t>
+  </si>
+  <si>
+    <t>SG PINT Credit Note v1.0</t>
+  </si>
+  <si>
+    <t>SG PINT Invoice v1.0</t>
+  </si>
+  <si>
+    <t>TICC-297</t>
   </si>
 </sst>
 </file>
@@ -2711,11 +2726,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F45987FB-91F4-488D-A9D3-2F3FAED3E07C}">
-  <dimension ref="A1:L243"/>
+  <dimension ref="A1:L245"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A230" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C241" sqref="C241"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A227" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K245" sqref="K245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10444,8 +10459,72 @@
         <v>130</v>
       </c>
     </row>
+    <row r="244" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A244" s="5" t="s">
+        <v>658</v>
+      </c>
+      <c r="B244" s="5" t="s">
+        <v>619</v>
+      </c>
+      <c r="C244" s="5" t="s">
+        <v>655</v>
+      </c>
+      <c r="D244" s="29" t="s">
+        <v>639</v>
+      </c>
+      <c r="E244" s="24" t="s">
+        <v>368</v>
+      </c>
+      <c r="H244" s="5" t="s">
+        <v>659</v>
+      </c>
+      <c r="I244" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J244" s="24">
+        <v>3</v>
+      </c>
+      <c r="K244" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="L244" s="5" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="245" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A245" s="5" t="s">
+        <v>657</v>
+      </c>
+      <c r="B245" s="5" t="s">
+        <v>619</v>
+      </c>
+      <c r="C245" s="5" t="s">
+        <v>656</v>
+      </c>
+      <c r="D245" s="29" t="s">
+        <v>639</v>
+      </c>
+      <c r="E245" s="24" t="s">
+        <v>368</v>
+      </c>
+      <c r="H245" s="5" t="s">
+        <v>659</v>
+      </c>
+      <c r="I245" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J245" s="24">
+        <v>3</v>
+      </c>
+      <c r="K245" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="L245" s="5" t="s">
+        <v>622</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:L237" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:L245" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>